<commit_message>
[WKS] more platforms added
</commit_message>
<xml_diff>
--- a/wks/WKS_platforma_robotyki.xlsx
+++ b/wks/WKS_platforma_robotyki.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
   <si>
     <t>fischertechnik ROBOTICS</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>ROBO Pro Software</t>
-  </si>
-  <si>
-    <t>inne modele</t>
-  </si>
-  <si>
-    <t>dużo</t>
   </si>
   <si>
     <t>http://www.fischertechnik.de/home/produkte/computing.aspx
@@ -86,32 +80,100 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>zumo</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/2509</t>
+  </si>
+  <si>
+    <t>Makeblock</t>
+  </si>
+  <si>
+    <t>http://www.makeblock.cc/starter-robot-kit-blue-bluetooth-version/
+https://www.youtube.com/watch?v=4WdDitRFxC0</t>
+  </si>
+  <si>
+    <t>różnorodność</t>
+  </si>
+  <si>
+    <t>mała</t>
+  </si>
+  <si>
+    <t>średnia</t>
+  </si>
+  <si>
+    <t>standardowe dla arduino</t>
+  </si>
+  <si>
+    <t>C/C++</t>
+  </si>
+  <si>
+    <t>standardowe dla arduino
+mBlock (Scratch)</t>
+  </si>
+  <si>
+    <t>LoFoRobot</t>
+  </si>
+  <si>
+    <t>http://www.lofirobot.com/</t>
+  </si>
+  <si>
+    <t>standardowe dla arduino
+Snap4Arduino</t>
+  </si>
+  <si>
+    <t>tak
+(dokupić czujniki)</t>
+  </si>
+  <si>
+    <t>niska</t>
+  </si>
+  <si>
+    <t>Podstawowy</t>
+  </si>
+  <si>
+    <t>http://www.lofirobot.com/produkt/zestaw-na-kolach/?attribute_bluetooth=bez-modulu-komunikacji-bezprzewodowej&amp;attribute_arduino=arduino-leonardo</t>
+  </si>
+  <si>
+    <t>http://botland.com.pl/pololu-zumo-robot/2937-zumo-v12-robot-minisumo-kit-dla-arduino.html
+http://botland.com.pl/arduino-moduly-glowne/1213-arduino-leonardo.html</t>
+  </si>
+  <si>
+    <t>Starter Robot Kit-Blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drewniane części
+</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>połączemie za pomocą kabelków i płytki stykowej</t>
+  </si>
+  <si>
+    <t>czyste arduino</t>
+  </si>
+  <si>
+    <t>specjalistyczna płytka (połączenie arduino i motor shield)
+wyspecjalizowane wejścia/wyjścia (http://wiki.makeblock.cc/index.php?title=Me-Baseboard)</t>
   </si>
   <si>
     <t>popularne (w Niemczech od &gt; 20 lat)
 wiele rozszerzeń
 solidnie wykonane
-mniej dziecinne (w porownaniu do lego)</t>
+mniej "dziecinne" (w porównaniu do lego)</t>
   </si>
   <si>
     <t>wolne silniki
-mało czujników w zestawie (ale można dokupić)</t>
-  </si>
-  <si>
-    <t>zumo</t>
-  </si>
-  <si>
-    <t>http://botland.com.pl/pololu-zumo-robot/2937-zumo-v12-robot-minisumo-kit-dla-arduino.html</t>
-  </si>
-  <si>
-    <t>https://www.pololu.com/product/2509</t>
-  </si>
-  <si>
-    <t>Makeblock</t>
-  </si>
-  <si>
-    <t>http://www.makeblock.cc/starter-robot-kit-blue-bluetooth-version/
-https://www.youtube.com/watch?v=4WdDitRFxC0</t>
+mało czujników w zestawie (można dokupić - drogie)</t>
+  </si>
+  <si>
+    <t>http://www.makeblock.cc/starter-robot-kit-blue-ir-version/
+http://www.trobot.pl/sklep/swiat-robotow/makeblock_zestaw_startowy_z_bluetooth_niebieski/
+http://www.exp-tech.de/robotik/makeblock/roboter-bausaetze/mechanische-bausaetze/makeblock-starter-robot-kit-v2-0-blue-with-electronics</t>
   </si>
 </sst>
 </file>
@@ -465,27 +527,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N5"/>
+  <dimension ref="A2:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
     <col min="2" max="2" width="65.140625" customWidth="1"/>
-    <col min="3" max="7" width="15" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="54.42578125" customWidth="1"/>
+    <col min="12" max="12" width="64.42578125" customWidth="1"/>
     <col min="13" max="13" width="43" customWidth="1"/>
     <col min="14" max="14" width="32.5703125" customWidth="1"/>
+    <col min="15" max="15" width="53.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +563,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -517,24 +581,27 @@
         <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L2" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="60">
+    <row r="3" spans="1:15" ht="60">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -543,10 +610,10 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
@@ -558,48 +625,157 @@
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <f>369.95 *4.17</f>
         <v>1542.6914999999999</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="60">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4">
+        <f>179+95</f>
+        <v>274</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="90">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5">
+        <f>3.7 * 150</f>
+        <v>555</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="6" spans="1:15" ht="30">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="30">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" t="s">
         <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6">
+        <v>500</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="http://www.fischertechnik.de/home/produkte/computing.aspx"/>
     <hyperlink ref="L3" r:id="rId2"/>
-    <hyperlink ref="L4" r:id="rId3"/>
+    <hyperlink ref="L4" r:id="rId3" display="http://botland.com.pl/pololu-zumo-robot/2937-zumo-v12-robot-minisumo-kit-dla-arduino.html"/>
     <hyperlink ref="B4" r:id="rId4"/>
     <hyperlink ref="B5" r:id="rId5" display="http://www.makeblock.cc/starter-robot-kit-blue-bluetooth-version/"/>
+    <hyperlink ref="B6" r:id="rId6"/>
+    <hyperlink ref="L6" r:id="rId7"/>
+    <hyperlink ref="L5" r:id="rId8" display="http://www.makeblock.cc/starter-robot-kit-blue-bluetooth-version/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>